<commit_message>
Motor speed Finally the same RPM
</commit_message>
<xml_diff>
--- a/Arduino/Arduino Project Timeline.xlsx
+++ b/Arduino/Arduino Project Timeline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/659c071ba0b66ebb/Documents/Nanyang Technological University/Semester 2 Year 20-21/Multidisciplinary Design Project (CE3004)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/659c071ba0b66ebb/Documents/GitHub/MDP-Group-10/Arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{5D9F51D7-97E5-4CB9-AF95-115F93F7E4E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B6FB0ADA-E402-43D5-9D54-DE5EF33E3868}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{5D9F51D7-97E5-4CB9-AF95-115F93F7E4E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D1139AC5-21DB-4E40-A68C-DC9FE6C8E171}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{7A5271F7-222A-4891-933D-2A67376D5F98}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>No</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Test Component Functionality</t>
   </si>
   <si>
-    <t>1 Day</t>
-  </si>
-  <si>
     <t>Assemble Robot Structure</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Able to travel in a straight line and steer 90 or 180 degrees.</t>
   </si>
   <si>
-    <t>Able to send text based messages to each other.</t>
-  </si>
-  <si>
     <t>Includes wiring kayout and strategic placement of sensors.</t>
   </si>
   <si>
@@ -100,6 +94,18 @@
   </si>
   <si>
     <t>To detect and successfully avoid obstacles when navigating.</t>
+  </si>
+  <si>
+    <t>2 Days</t>
+  </si>
+  <si>
+    <t>Able to send text based messages to each other over serial.</t>
+  </si>
+  <si>
+    <t>5 Days</t>
+  </si>
+  <si>
+    <t>3 Days</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561BAC32-5CAD-4D48-9768-6BD5860AA898}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -531,16 +537,16 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3">
         <v>44212</v>
       </c>
       <c r="G2" s="3">
-        <v>44212</v>
+        <v>44213</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -554,19 +560,19 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3">
-        <v>44213</v>
+        <v>44214</v>
       </c>
       <c r="G3" s="3">
-        <v>44213</v>
+        <v>44215</v>
       </c>
       <c r="H3" s="1">
         <v>2</v>
@@ -580,14 +586,20 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44216</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44217</v>
+      </c>
       <c r="H4" s="1">
         <v>3</v>
       </c>
@@ -600,14 +612,20 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44218</v>
+      </c>
+      <c r="G5" s="3">
+        <v>44222</v>
+      </c>
       <c r="H5" s="1">
         <v>4</v>
       </c>
@@ -620,14 +638,20 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44223</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44225</v>
+      </c>
       <c r="H6" s="1">
         <v>5</v>
       </c>
@@ -640,15 +664,23 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="F7" s="3">
+        <v>44226</v>
+      </c>
+      <c r="G7" s="3">
+        <v>44227</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -706,6 +738,76 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>